<commit_message>
Completed the the CF renaming function. Only support first plate.
</commit_message>
<xml_diff>
--- a/demoSamples/renamingCF.xlsx
+++ b/demoSamples/renamingCF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yiton\Documents\PyCodes\EasyFlowQ3\demoSamples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yiton\Documents\PyCodes\EasyFlowQ\demoSamples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265653AC-2C47-4A6D-ADAA-C2D164133C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8F5ED5-3951-45B3-9783-E68A89626DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24850" windowHeight="16220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="290" windowWidth="18390" windowHeight="11710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="13">
   <si>
     <t>smpl1</t>
   </si>
@@ -51,6 +51,21 @@
   </si>
   <si>
     <t>smpl8</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>unique2</t>
+  </si>
+  <si>
+    <t>uniquex</t>
+  </si>
+  <si>
+    <t>uniquex1</t>
+  </si>
+  <si>
+    <t>uniquex3</t>
   </si>
 </sst>
 </file>
@@ -374,26 +389,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -413,16 +428,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
@@ -442,22 +457,22 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -471,16 +486,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -500,16 +515,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -528,17 +543,14 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -557,17 +569,14 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -580,17 +589,14 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -599,6 +605,50 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -845,10 +895,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA705DE4-3873-444E-9B82-5FD8C2247234}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -963,7 +1013,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -972,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
@@ -1115,6 +1165,90 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>